<commit_message>
My first FLask apps
</commit_message>
<xml_diff>
--- a/pokemonitems.xlsx
+++ b/pokemonitems.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,238 +443,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>master-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ultra-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>great-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>poke-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>safari-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>net-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>dive-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>nest-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>repeat-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>timer-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>luxury-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>premier-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>dusk-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>heal-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>quick-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>cherish-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>smoke-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>light-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>iron-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>lure-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>level-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>moon-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>heavy-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>fast-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>friend-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>love-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>park-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>sport-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>air-balloon</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>dream-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>snowball</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>beast-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>left-poke-ball</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>polished-mud-ball</t>
+          <t>slowbronite</t>
         </is>
       </c>
     </row>

</xml_diff>